<commit_message>
thresholded and ran AN's data, added in tuned overlap code to tuning_analysis, created troubleshooting code from David
still trying to figure out how to create a venn diagram
</commit_message>
<xml_diff>
--- a/ExcelFiles/s2_good_trials_GraspObject_Shuffled.xlsx
+++ b/ExcelFiles/s2_good_trials_GraspObject_Shuffled.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macthurston\Documents\GitHub\project_grasp_object_interaction\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00ECA3A1-AF9C-45C0-89E5-7BAE8A235AC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B2AC937-964C-4ED7-B4FE-71686C4594E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="990" yWindow="300" windowWidth="14115" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-3135" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -44,6 +44,18 @@
   </si>
   <si>
     <t>15,23</t>
+  </si>
+  <si>
+    <t>11,15,18</t>
+  </si>
+  <si>
+    <t>8,10,18</t>
+  </si>
+  <si>
+    <t>7,18,24</t>
+  </si>
+  <si>
+    <t>9,10,16</t>
   </si>
 </sst>
 </file>
@@ -362,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,6 +459,46 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>20240216</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
a lot of edits!!
I've been bad about pushing so I need to get better about that. Changes include:
-saving analyzed data as mat files
-updated excel files for all sessions run with participants
-updated grasp_decoding for varied_sizes
-updated pixelated_tuning analysis
-updated firing_rates and tuning_analysis to analyze varied_sizes
-MCN decoder
</commit_message>
<xml_diff>
--- a/ExcelFiles/s2_good_trials_GraspObject_Shuffled.xlsx
+++ b/ExcelFiles/s2_good_trials_GraspObject_Shuffled.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macthurston\Documents\GitHub\project_grasp_object_interaction\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B2AC937-964C-4ED7-B4FE-71686C4594E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF670491-ED64-4BD6-8AD3-71C61A8086FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-3135" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3255" yWindow="2910" windowWidth="12150" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -56,6 +56,57 @@
   </si>
   <si>
     <t>9,10,16</t>
+  </si>
+  <si>
+    <t>10,11,12,18,22,23,24</t>
+  </si>
+  <si>
+    <t>6,7,10,11,15,18,19,22,23,24</t>
+  </si>
+  <si>
+    <t>7,11,14,18,19,22,23,24</t>
+  </si>
+  <si>
+    <t>4,5,6,12,16,19</t>
+  </si>
+  <si>
+    <t>6,13,20,23</t>
+  </si>
+  <si>
+    <t>12,22,23</t>
+  </si>
+  <si>
+    <t>8,20</t>
+  </si>
+  <si>
+    <t>6,7</t>
+  </si>
+  <si>
+    <t>15,24</t>
+  </si>
+  <si>
+    <t>2,6,10,17,22</t>
+  </si>
+  <si>
+    <t>19,23</t>
+  </si>
+  <si>
+    <t>17,18,23</t>
+  </si>
+  <si>
+    <t>11,17,21,23,24</t>
+  </si>
+  <si>
+    <t>16,22</t>
+  </si>
+  <si>
+    <t>5,9,14</t>
+  </si>
+  <si>
+    <t>10,24</t>
+  </si>
+  <si>
+    <t>not included bc bad session</t>
   </si>
 </sst>
 </file>
@@ -374,21 +425,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="31.42578125" customWidth="1"/>
-    <col min="5" max="5" width="29.42578125" customWidth="1"/>
-    <col min="6" max="6" width="38.140625" customWidth="1"/>
-    <col min="7" max="7" width="27" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -499,6 +550,169 @@
         <v>12</v>
       </c>
     </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>20240625</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>21</v>
+      </c>
+      <c r="F8">
+        <v>22</v>
+      </c>
+      <c r="G8">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>20240703</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>20240710</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>20240716</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated tuning analysis to save desired values
updated tuning analysis to rerun everything and save desired values for future analyses. Updated participant sessions
</commit_message>
<xml_diff>
--- a/ExcelFiles/s2_good_trials_GraspObject_Shuffled.xlsx
+++ b/ExcelFiles/s2_good_trials_GraspObject_Shuffled.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macthurston\Documents\GitHub\project_grasp_object_interaction\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF670491-ED64-4BD6-8AD3-71C61A8086FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231FBC40-0718-4749-8D1C-8D91B1401333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3255" yWindow="2910" windowWidth="12150" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="22920" windowHeight="13230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>not included bc bad session</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
   </si>
 </sst>
 </file>
@@ -425,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,6 +716,108 @@
         <v>26</v>
       </c>
     </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>20241023</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>20241028</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <v>3</v>
+      </c>
+      <c r="G17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>20241111</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>6</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20250120</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>5</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>